<commit_message>
validación de suma asegurada cotización y emisión
</commit_message>
<xml_diff>
--- a/Sura/Validación de Suma Asegurada - Emisión.xlsx
+++ b/Sura/Validación de Suma Asegurada - Emisión.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Downloads\Sura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA56F385-423F-4E64-B7FF-A4DE110BDA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4353B4EE-ED97-44A8-BDE6-2F036BB93BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="57">
   <si>
     <t>Usuario</t>
   </si>
@@ -178,13 +178,31 @@
   </si>
   <si>
     <t>13.000.000</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
+  </si>
+  <si>
+    <t>gw</t>
+  </si>
+  <si>
+    <t>3582596139</t>
+  </si>
+  <si>
+    <t>7.000.000</t>
+  </si>
+  <si>
+    <t>9.000.000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -218,6 +236,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF232323"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -249,6 +273,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -532,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,13 +897,129 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="E7" s="4"/>
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6">
+        <v>2022</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7">
+        <v>2022</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>

</xml_diff>

<commit_message>
validacion suma asegurada sin bloqueo
</commit_message>
<xml_diff>
--- a/Sura/Validación de Suma Asegurada - Emisión.xlsx
+++ b/Sura/Validación de Suma Asegurada - Emisión.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4353B4EE-ED97-44A8-BDE6-2F036BB93BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8566B5C9-BEED-4E63-ACF3-B444FA55A85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
   <si>
     <t>Usuario</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>9.000.000</t>
+  </si>
+  <si>
+    <t>Validacion</t>
+  </si>
+  <si>
+    <t>5.000.000</t>
   </si>
 </sst>
 </file>
@@ -264,12 +270,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -558,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9:T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,13 +691,13 @@
       <c r="M2">
         <v>2021</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>47</v>
       </c>
       <c r="Q2" t="s">
@@ -748,13 +753,13 @@
       <c r="M3">
         <v>2021</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>47</v>
       </c>
       <c r="Q3" t="s">
@@ -810,13 +815,13 @@
       <c r="M4">
         <v>2021</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>50</v>
       </c>
       <c r="Q4" t="s">
@@ -872,13 +877,13 @@
       <c r="M5">
         <v>2021</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>50</v>
       </c>
       <c r="Q5" t="s">
@@ -910,7 +915,7 @@
       <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F6" t="s">
@@ -934,13 +939,13 @@
       <c r="M6">
         <v>2022</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="6" t="s">
         <v>56</v>
       </c>
       <c r="Q6" t="s">
@@ -972,7 +977,7 @@
       <c r="D7" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F7" t="s">
@@ -996,13 +1001,13 @@
       <c r="M7">
         <v>2022</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="6" t="s">
         <v>55</v>
       </c>
       <c r="Q7" t="s">
@@ -1021,9 +1026,67 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="E8" s="4"/>
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8">
+        <v>2022</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" t="s">
+        <v>44</v>
+      </c>
+      <c r="U8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>

</xml_diff>